<commit_message>
oct avoid with 09/30 data
</commit_message>
<xml_diff>
--- a/data/octanol_30pct_avoidance_210827.xlsx
+++ b/data/octanol_30pct_avoidance_210827.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friv\git\cest-2.1-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\friv\git\cest-2.1-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59839AE3-A0F3-405F-B760-426C4E967AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B703077-1276-4EAA-AB1F-B01C55AAE7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DB5CA776-E608-47C3-9A1B-07ACB9CEE812}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>N2</t>
   </si>
   <si>
-    <t>30pct_oct</t>
-  </si>
-  <si>
     <t>MOD</t>
   </si>
   <si>
@@ -65,11 +62,17 @@
   <si>
     <t>cest-2.1</t>
   </si>
+  <si>
+    <t>30pct</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +110,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,14 +427,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16BCBE5-C5EC-48BF-B884-694DC38675CA}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49:E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -456,13 +459,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>2.4</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1">
         <v>44435</v>
@@ -473,13 +476,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>1.5</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1">
         <v>44435</v>
@@ -490,13 +493,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1.31</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1">
         <v>44435</v>
@@ -507,13 +510,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>4.1500000000000004</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1">
         <v>44435</v>
@@ -524,13 +527,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>3.39</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1">
         <v>44435</v>
@@ -541,13 +544,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2.97</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="1">
         <v>44435</v>
@@ -558,13 +561,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>2.42</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="1">
         <v>44435</v>
@@ -575,13 +578,13 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>3.72</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1">
         <v>44435</v>
@@ -592,13 +595,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>4.16</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1">
         <v>44435</v>
@@ -609,13 +612,13 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>1.8</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1">
         <v>44435</v>
@@ -626,13 +629,13 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>3.8</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="1">
         <v>44435</v>
@@ -643,13 +646,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>1.4</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <v>44435</v>
@@ -660,13 +663,13 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>1.8</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1">
         <v>44435</v>
@@ -677,13 +680,13 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>1.3</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <v>44435</v>
@@ -694,13 +697,13 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>3.04</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1">
         <v>44435</v>
@@ -711,13 +714,13 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>1.9</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1">
         <v>44435</v>
@@ -728,13 +731,13 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>1.1000000000000001</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="1">
         <v>44435</v>
@@ -745,13 +748,13 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>1.6</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>44435</v>
@@ -762,13 +765,13 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>1.4</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1">
         <v>44435</v>
@@ -779,13 +782,13 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>2.2000000000000002</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="1">
         <v>44435</v>
@@ -793,16 +796,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>2.5</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="1">
         <v>44435</v>
@@ -810,16 +813,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <v>6.24</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1">
         <v>44435</v>
@@ -827,16 +830,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>5.58</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1">
         <v>44435</v>
@@ -844,16 +847,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>1.93</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
         <v>44435</v>
@@ -861,16 +864,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>2.58</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1">
         <v>44435</v>
@@ -878,16 +881,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>4.1500000000000004</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1">
         <v>44435</v>
@@ -895,16 +898,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>2.92</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="1">
         <v>44435</v>
@@ -912,16 +915,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>6.98</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="1">
         <v>44435</v>
@@ -929,16 +932,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <v>1.23</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1">
         <v>44435</v>
@@ -946,16 +949,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>2.56</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="1">
         <v>44435</v>
@@ -963,16 +966,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>3.9</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" s="1">
         <v>44435</v>
@@ -980,16 +983,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>1.2</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="1">
         <v>44435</v>
@@ -997,16 +1000,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>1.9</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" s="1">
         <v>44435</v>
@@ -1014,16 +1017,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C35">
         <v>9.6</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1">
         <v>44435</v>
@@ -1031,16 +1034,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C36">
         <v>1.4</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1">
         <v>44435</v>
@@ -1048,16 +1051,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <v>1.8</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E37" s="1">
         <v>44435</v>
@@ -1065,16 +1068,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>2.5</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1">
         <v>44435</v>
@@ -1082,16 +1085,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C39">
         <v>4.3</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="1">
         <v>44435</v>
@@ -1099,16 +1102,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C40">
         <v>1.8</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" s="1">
         <v>44435</v>
@@ -1116,16 +1119,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C41">
         <v>1.1000000000000001</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="1">
         <v>44435</v>
@@ -1136,13 +1139,13 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C42">
         <v>1.17</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42" s="1">
         <v>44435</v>
@@ -1153,13 +1156,13 @@
         <v>5</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>3.14</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43" s="1">
         <v>44435</v>
@@ -1170,13 +1173,13 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C44">
         <v>4.07</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1">
         <v>44435</v>
@@ -1187,13 +1190,13 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C45">
         <v>3.21</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45" s="1">
         <v>44435</v>
@@ -1204,13 +1207,13 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>2.33</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46" s="1">
         <v>44435</v>
@@ -1221,13 +1224,13 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C47">
         <v>1.25</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E47" s="1">
         <v>44435</v>
@@ -1238,13 +1241,13 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C48">
         <v>1.79</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E48" s="1">
         <v>44435</v>
@@ -1255,13 +1258,13 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>2.98</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E49" s="1">
         <v>44435</v>
@@ -1269,16 +1272,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C50">
         <v>2.6</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50" s="1">
         <v>44435</v>
@@ -1286,16 +1289,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C51">
         <v>3.8</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E51" s="1">
         <v>44435</v>
@@ -1303,16 +1306,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C52">
         <v>1.5</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E52" s="1">
         <v>44435</v>
@@ -1320,16 +1323,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C53">
         <v>1.3</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1">
         <v>44435</v>
@@ -1337,16 +1340,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C54">
         <v>2.9</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1">
         <v>44435</v>
@@ -1354,16 +1357,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C55">
         <v>1.5</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E55" s="1">
         <v>44435</v>
@@ -1371,16 +1374,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C56">
         <v>2.2999999999999998</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56" s="1">
         <v>44435</v>
@@ -1388,16 +1391,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C57">
         <v>1.8</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="1">
         <v>44435</v>
@@ -1405,16 +1408,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B58" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C58">
         <v>3.6</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E58" s="1">
         <v>44435</v>
@@ -1422,16 +1425,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>1.3</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E59" s="1">
         <v>44435</v>

</xml_diff>